<commit_message>
feat(difftool): add difftool wrapper, supporting only diffmerge
</commit_message>
<xml_diff>
--- a/src/test/data/the-attorney.xlsx
+++ b/src/test/data/the-attorney.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pismute\git\node-textconv\src\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="0" windowWidth="22140" windowHeight="12672"/>
+    <workbookView xWindow="20" yWindow="80" windowWidth="22340" windowHeight="17560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="staff" sheetId="1" r:id="rId1"/>
     <sheet name="cast" sheetId="2" r:id="rId2"/>
+    <sheet name="description" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Director</t>
   </si>
@@ -79,19 +78,27 @@
   </si>
   <si>
     <t>staff</t>
+  </si>
+  <si>
+    <t>An ambitious tax attorney decides to represent an old friend in court.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF333333"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,8 +121,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -176,7 +184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -211,7 +219,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -388,7 +396,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -398,22 +406,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -421,7 +429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -434,7 +442,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -446,18 +458,18 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -465,7 +477,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -473,7 +485,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3">
       <c r="B4" t="s">
         <v>9</v>
       </c>
@@ -481,7 +493,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3">
       <c r="B5" t="s">
         <v>11</v>
       </c>
@@ -489,7 +501,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3">
       <c r="B6" t="s">
         <v>13</v>
       </c>
@@ -497,7 +509,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3">
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -507,5 +519,35 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="2:2" ht="17">
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>